<commit_message>
I don't know what I did.
</commit_message>
<xml_diff>
--- a/Hardware/ATmegaXXM1_Breakout.xlsx
+++ b/Hardware/ATmegaXXM1_Breakout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="105">
   <si>
     <t>Reference</t>
   </si>
@@ -316,6 +316,24 @@
   </si>
   <si>
     <t>PANASONIC</t>
+  </si>
+  <si>
+    <t>SH1 SH2 SH3</t>
+  </si>
+  <si>
+    <t>JUMPER</t>
+  </si>
+  <si>
+    <t>2 (1 x 2) Position Shunt Connector Black Open Top 0.100" (2.54mm) Gold</t>
+  </si>
+  <si>
+    <t>969102-0000-DA</t>
+  </si>
+  <si>
+    <t>3M9580-ND</t>
+  </si>
+  <si>
+    <t>QTY (x25)</t>
   </si>
 </sst>
 </file>
@@ -866,18 +884,22 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -893,14 +915,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:J17" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="B2:J17"/>
-  <tableColumns count="9">
-    <tableColumn id="9" name="Line Number" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:K18" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="B2:K18"/>
+  <tableColumns count="10">
+    <tableColumn id="9" name="Line Number" dataDxfId="3"/>
     <tableColumn id="1" name="Reference"/>
     <tableColumn id="2" name="QTY"/>
-    <tableColumn id="4" name=" Value" dataDxfId="3"/>
-    <tableColumn id="7" name="Description" dataDxfId="2"/>
+    <tableColumn id="10" name="QTY (x25)" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[QTY]]*25</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name=" Value" dataDxfId="2"/>
+    <tableColumn id="7" name="Description" dataDxfId="1"/>
     <tableColumn id="5" name=" Footprint"/>
     <tableColumn id="3" name="MFG"/>
     <tableColumn id="6" name=" MFG#"/>
@@ -1207,10 +1232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J17"/>
+  <dimension ref="B2:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,19 +1243,19 @@
     <col min="1" max="1" width="3.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="77" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1"/>
-    <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" customWidth="1"/>
-    <col min="13" max="13" width="28.42578125" customWidth="1"/>
-    <col min="14" max="14" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="7" max="7" width="77" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" customWidth="1"/>
+    <col min="14" max="14" width="28.42578125" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>44</v>
       </c>
@@ -1241,25 +1266,28 @@
         <v>38</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -1269,26 +1297,30 @@
       <c r="D3" s="3">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>100</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>86</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>87</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -1298,26 +1330,30 @@
       <c r="D4" s="3">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>50</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>47</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>46</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -1327,26 +1363,30 @@
       <c r="D5" s="3">
         <v>2</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>50</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>47</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>89</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>4</v>
       </c>
@@ -1356,26 +1396,30 @@
       <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>50</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>52</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>50</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>5</v>
       </c>
@@ -1385,26 +1429,30 @@
       <c r="D7" s="3">
         <v>2</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>50</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>80</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>18</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>6</v>
       </c>
@@ -1414,26 +1462,30 @@
       <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>25</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>75</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>76</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>7</v>
       </c>
@@ -1443,26 +1495,30 @@
       <c r="D9" s="3">
         <v>1</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>25</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>77</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>83</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>81</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>8</v>
       </c>
@@ -1472,26 +1528,30 @@
       <c r="D10" s="3">
         <v>2</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>50</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>64</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>65</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>9</v>
       </c>
@@ -1501,26 +1561,30 @@
       <c r="D11" s="3">
         <v>2</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>50</v>
+      </c>
+      <c r="F11" s="1">
         <v>470</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>64</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>6</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>10</v>
       </c>
@@ -1530,26 +1594,30 @@
       <c r="D12" s="3">
         <v>1</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>25</v>
+      </c>
+      <c r="F12" s="1">
         <v>120</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>64</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>69</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>11</v>
       </c>
@@ -1559,24 +1627,28 @@
       <c r="D13" s="3">
         <v>1</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>25</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" t="s">
+      <c r="H13" s="2"/>
+      <c r="I13" t="s">
         <v>98</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>96</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>12</v>
       </c>
@@ -1586,26 +1658,30 @@
       <c r="D14" s="3">
         <v>1</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>25</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>33</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>40</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>13</v>
       </c>
@@ -1615,26 +1691,30 @@
       <c r="D15" s="3">
         <v>1</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>25</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>57</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>55</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>14</v>
       </c>
@@ -1644,24 +1724,28 @@
       <c r="D16" s="3">
         <v>1</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>25</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" t="s">
+      <c r="H16" s="2"/>
+      <c r="I16" t="s">
         <v>33</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>61</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="K16" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>15</v>
       </c>
@@ -1671,23 +1755,58 @@
       <c r="D17" s="3">
         <v>1</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>25</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>72</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>13</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3">
+        <f>Table1[[#This Row],[QTY]]*25</f>
+        <v>75</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" t="s">
+        <v>102</v>
+      </c>
+      <c r="K18" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>